<commit_message>
functions added in search page
</commit_message>
<xml_diff>
--- a/store/data.xlsx
+++ b/store/data.xlsx
@@ -684,7 +684,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -888,27 +888,6 @@
       </c>
       <c r="E9" s="2" t="n">
         <v>6463464364</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>sdfas</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>124214</v>
-      </c>
-      <c r="E10" t="n">
-        <v>332325325</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added date section and minor bug fixed
</commit_message>
<xml_diff>
--- a/store/data.xlsx
+++ b/store/data.xlsx
@@ -19,7 +19,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -39,6 +39,11 @@
     <font>
       <name val="Arial"/>
       <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
       <sz val="10"/>
     </font>
   </fonts>
@@ -69,17 +74,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,214 +466,214 @@
       <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col width="11.71" customWidth="1" style="2" min="1" max="64"/>
+    <col width="11.71" customWidth="1" style="3" min="1" max="64"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12.8" customHeight="1" s="3">
-      <c r="A1" s="2" t="inlineStr">
+    <row r="1" ht="12.8" customHeight="1" s="4">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>S.N</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>Rate</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>Availabe</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="12.8" customHeight="1" s="3">
-      <c r="A2" s="2" t="n">
+    <row r="2" ht="12.8" customHeight="1" s="4">
+      <c r="A2" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="inlineStr">
+      <c r="B2" s="3" t="inlineStr">
         <is>
           <t>Chickens</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="C2" s="3" t="inlineStr">
         <is>
           <t>300 Per KG</t>
         </is>
       </c>
-      <c r="D2" s="2" t="inlineStr">
+      <c r="D2" s="3" t="inlineStr">
         <is>
           <t>12 KG</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="12.8" customHeight="1" s="3">
-      <c r="A3" s="2" t="n">
+    <row r="3" ht="12.8" customHeight="1" s="4">
+      <c r="A3" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="inlineStr">
+      <c r="B3" s="3" t="inlineStr">
         <is>
           <t>Eggs</t>
         </is>
       </c>
-      <c r="C3" s="2" t="inlineStr">
+      <c r="C3" s="3" t="inlineStr">
         <is>
           <t>400 Per Crate</t>
         </is>
       </c>
-      <c r="D3" s="2" t="inlineStr">
+      <c r="D3" s="3" t="inlineStr">
         <is>
           <t>2000 Units</t>
         </is>
       </c>
     </row>
-    <row r="4" ht="12.8" customHeight="1" s="3">
-      <c r="A4" s="2" t="n">
+    <row r="4" ht="12.8" customHeight="1" s="4">
+      <c r="A4" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="inlineStr">
+      <c r="B4" s="3" t="inlineStr">
         <is>
           <t>Fish</t>
         </is>
       </c>
-      <c r="C4" s="2" t="inlineStr">
+      <c r="C4" s="3" t="inlineStr">
         <is>
           <t>300 Per KG</t>
         </is>
       </c>
-      <c r="D4" s="2" t="inlineStr">
+      <c r="D4" s="3" t="inlineStr">
         <is>
           <t>20 KG</t>
         </is>
       </c>
     </row>
-    <row r="5" ht="12.8" customHeight="1" s="3">
-      <c r="A5" s="2" t="n">
+    <row r="5" ht="12.8" customHeight="1" s="4">
+      <c r="A5" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="inlineStr">
+      <c r="B5" s="3" t="inlineStr">
         <is>
           <t>Chickens</t>
         </is>
       </c>
-      <c r="C5" s="2" t="inlineStr">
+      <c r="C5" s="3" t="inlineStr">
         <is>
           <t>300 Per KG</t>
         </is>
       </c>
-      <c r="D5" s="2" t="inlineStr">
+      <c r="D5" s="3" t="inlineStr">
         <is>
           <t>12 KG</t>
         </is>
       </c>
     </row>
-    <row r="6" ht="12.8" customHeight="1" s="3">
-      <c r="A6" s="2" t="n">
+    <row r="6" ht="12.8" customHeight="1" s="4">
+      <c r="A6" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="inlineStr">
+      <c r="B6" s="3" t="inlineStr">
         <is>
           <t>Eggs</t>
         </is>
       </c>
-      <c r="C6" s="2" t="inlineStr">
+      <c r="C6" s="3" t="inlineStr">
         <is>
           <t>400 Per Crate</t>
         </is>
       </c>
-      <c r="D6" s="2" t="inlineStr">
+      <c r="D6" s="3" t="inlineStr">
         <is>
           <t>2000 Units</t>
         </is>
       </c>
     </row>
-    <row r="7" ht="12.8" customHeight="1" s="3">
-      <c r="A7" s="2" t="n">
+    <row r="7" ht="12.8" customHeight="1" s="4">
+      <c r="A7" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="inlineStr">
+      <c r="B7" s="3" t="inlineStr">
         <is>
           <t>Fish</t>
         </is>
       </c>
-      <c r="C7" s="2" t="inlineStr">
+      <c r="C7" s="3" t="inlineStr">
         <is>
           <t>300 Per KG</t>
         </is>
       </c>
-      <c r="D7" s="2" t="inlineStr">
+      <c r="D7" s="3" t="inlineStr">
         <is>
           <t>20 KG</t>
         </is>
       </c>
     </row>
-    <row r="8" ht="12.8" customHeight="1" s="3">
-      <c r="A8" s="2" t="n">
+    <row r="8" ht="12.8" customHeight="1" s="4">
+      <c r="A8" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="inlineStr">
+      <c r="B8" s="3" t="inlineStr">
         <is>
           <t>Chickens</t>
         </is>
       </c>
-      <c r="C8" s="2" t="inlineStr">
+      <c r="C8" s="3" t="inlineStr">
         <is>
           <t>300 Per KG</t>
         </is>
       </c>
-      <c r="D8" s="2" t="inlineStr">
+      <c r="D8" s="3" t="inlineStr">
         <is>
           <t>12 KG</t>
         </is>
       </c>
     </row>
-    <row r="9" ht="12.8" customHeight="1" s="3">
-      <c r="A9" s="2" t="n">
+    <row r="9" ht="12.8" customHeight="1" s="4">
+      <c r="A9" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="inlineStr">
+      <c r="B9" s="3" t="inlineStr">
         <is>
           <t>Eggs</t>
         </is>
       </c>
-      <c r="C9" s="2" t="inlineStr">
+      <c r="C9" s="3" t="inlineStr">
         <is>
           <t>400 Per Crate</t>
         </is>
       </c>
-      <c r="D9" s="2" t="inlineStr">
+      <c r="D9" s="3" t="inlineStr">
         <is>
           <t>2000 Units</t>
         </is>
       </c>
     </row>
-    <row r="10" ht="12.8" customHeight="1" s="3">
-      <c r="A10" s="2" t="n">
+    <row r="10" ht="12.8" customHeight="1" s="4">
+      <c r="A10" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="inlineStr">
+      <c r="B10" s="3" t="inlineStr">
         <is>
           <t>Fish</t>
         </is>
       </c>
-      <c r="C10" s="2" t="inlineStr">
+      <c r="C10" s="3" t="inlineStr">
         <is>
           <t>300 Per KG</t>
         </is>
       </c>
-      <c r="D10" s="2" t="inlineStr">
+      <c r="D10" s="3" t="inlineStr">
         <is>
           <t>20 KG</t>
         </is>
       </c>
     </row>
-    <row r="11" ht="12.8" customHeight="1" s="3"/>
+    <row r="11" ht="12.8" customHeight="1" s="4"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -684,212 +695,941 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col width="11.69" customWidth="1" style="2" min="1" max="64"/>
+    <col width="11.69" customWidth="1" style="3" min="1" max="5"/>
+    <col width="19.02" customWidth="1" style="3" min="6" max="6"/>
+    <col width="11.69" customWidth="1" style="3" min="7" max="64"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12.8" customHeight="1" s="3">
-      <c r="A1" s="2" t="inlineStr">
+    <row r="1" ht="12.8" customHeight="1" s="4">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>S.N</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>Phone No</t>
         </is>
       </c>
-    </row>
-    <row r="2" ht="12.8" customHeight="1" s="3">
-      <c r="A2" s="2" t="n">
+      <c r="F1" s="3" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="12.8" customHeight="1" s="4">
+      <c r="A2" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>Akshita</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="inlineStr">
-        <is>
-          <t>Paint</t>
-        </is>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>2000</v>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>9845069988</v>
-      </c>
-    </row>
-    <row r="3" ht="12.8" customHeight="1" s="3">
-      <c r="A3" s="2" t="n">
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>Akshita</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>Paint</t>
+        </is>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>9845069988</v>
+      </c>
+      <c r="F2" s="3" t="inlineStr">
+        <is>
+          <t>2020-08-01;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="12.8" customHeight="1" s="4">
+      <c r="A3" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="inlineStr">
+      <c r="B3" s="3" t="inlineStr">
         <is>
           <t>Aakash</t>
         </is>
       </c>
-      <c r="C3" s="2" t="inlineStr">
+      <c r="C3" s="3" t="inlineStr">
         <is>
           <t>Grains</t>
         </is>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="D3" s="3" t="n">
         <v>1000</v>
       </c>
-      <c r="E3" s="2" t="n">
+      <c r="E3" s="3" t="n">
         <v>9847081990</v>
       </c>
-    </row>
-    <row r="4" ht="12.8" customHeight="1" s="3">
-      <c r="A4" s="2" t="n">
+      <c r="F3" s="3" t="inlineStr">
+        <is>
+          <t>2020-08-01;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="12.8" customHeight="1" s="4">
+      <c r="A4" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>Akshita</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>Paint</t>
-        </is>
-      </c>
-      <c r="D4" s="2" t="n">
-        <v>2000</v>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>9845069988</v>
-      </c>
-    </row>
-    <row r="5" ht="12.8" customHeight="1" s="3">
-      <c r="A5" s="2" t="n">
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>Akshita</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>Paint</t>
+        </is>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>9845069988</v>
+      </c>
+      <c r="F4" s="3" t="inlineStr">
+        <is>
+          <t>2020-08-01;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="12.8" customHeight="1" s="4">
+      <c r="A5" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="inlineStr">
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>aakash</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>fish</t>
+        </is>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>10000000</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>9847081990</v>
+      </c>
+      <c r="F5" s="3" t="inlineStr">
+        <is>
+          <t>2020-08-01;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="12.8" customHeight="1" s="4">
+      <c r="A6" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>Akshita</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="inlineStr">
+        <is>
+          <t>Paint</t>
+        </is>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>9845069988</v>
+      </c>
+      <c r="F6" s="3" t="inlineStr">
+        <is>
+          <t>2020-08-01;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="12.8" customHeight="1" s="4">
+      <c r="A7" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
         <is>
           <t>Aakash</t>
         </is>
       </c>
-      <c r="C5" s="2" t="inlineStr">
+      <c r="C7" s="3" t="inlineStr">
         <is>
           <t>Grains</t>
         </is>
       </c>
-      <c r="D5" s="2" t="n">
+      <c r="D7" s="3" t="n">
         <v>1000</v>
       </c>
-      <c r="E5" s="2" t="n">
+      <c r="E7" s="3" t="n">
         <v>9847081990</v>
       </c>
-    </row>
-    <row r="6" ht="12.8" customHeight="1" s="3">
-      <c r="A6" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="inlineStr">
-        <is>
-          <t>Akshita</t>
-        </is>
-      </c>
-      <c r="C6" s="2" t="inlineStr">
-        <is>
-          <t>Paint</t>
-        </is>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>2000</v>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>9845069988</v>
-      </c>
-    </row>
-    <row r="7" ht="12.8" customHeight="1" s="3">
-      <c r="A7" s="2" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="inlineStr">
+      <c r="F7" s="3" t="inlineStr">
+        <is>
+          <t>2020-08-02;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="12.8" customHeight="1" s="4">
+      <c r="A8" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="inlineStr">
+        <is>
+          <t>Akshita</t>
+        </is>
+      </c>
+      <c r="C8" s="3" t="inlineStr">
+        <is>
+          <t>Paint</t>
+        </is>
+      </c>
+      <c r="D8" s="3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E8" s="3" t="n">
+        <v>9845069988</v>
+      </c>
+      <c r="F8" s="3" t="inlineStr">
+        <is>
+          <t>2020-08-02;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="12.8" customHeight="1" s="4">
+      <c r="A9" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>aakash</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>fish</t>
+        </is>
+      </c>
+      <c r="D9" s="3" t="n">
+        <v>10000000</v>
+      </c>
+      <c r="E9" s="3" t="n">
+        <v>9847081990</v>
+      </c>
+      <c r="F9" s="3" t="inlineStr">
+        <is>
+          <t>2020-08-02;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" ht="12.8" customHeight="1" s="4">
+      <c r="A10" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>Akshita</t>
+        </is>
+      </c>
+      <c r="C10" s="3" t="inlineStr">
+        <is>
+          <t>Paint</t>
+        </is>
+      </c>
+      <c r="D10" s="3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E10" s="3" t="n">
+        <v>9845069988</v>
+      </c>
+      <c r="F10" s="3" t="inlineStr">
+        <is>
+          <t>2020-08-03;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" ht="12.8" customHeight="1" s="4">
+      <c r="A11" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="inlineStr">
         <is>
           <t>Aakash</t>
         </is>
       </c>
-      <c r="C7" s="2" t="inlineStr">
+      <c r="C11" s="3" t="inlineStr">
         <is>
           <t>Grains</t>
         </is>
       </c>
-      <c r="D7" s="2" t="n">
+      <c r="D11" s="3" t="n">
         <v>1000</v>
       </c>
-      <c r="E7" s="2" t="n">
+      <c r="E11" s="3" t="n">
         <v>9847081990</v>
       </c>
-    </row>
-    <row r="8" ht="12.8" customHeight="1" s="3">
-      <c r="A8" s="2" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="inlineStr">
+      <c r="F11" s="3" t="inlineStr">
+        <is>
+          <t>2020-08-03;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" ht="12.8" customHeight="1" s="4">
+      <c r="A12" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>Akshita</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="inlineStr">
+        <is>
+          <t>Paint</t>
+        </is>
+      </c>
+      <c r="D12" s="3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E12" s="3" t="n">
+        <v>9845069988</v>
+      </c>
+      <c r="F12" s="3" t="inlineStr">
+        <is>
+          <t>2020-08-03;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="13" ht="12.8" customHeight="1" s="4">
+      <c r="A13" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="inlineStr">
+        <is>
+          <t>Akshita</t>
+        </is>
+      </c>
+      <c r="C13" s="3" t="inlineStr">
+        <is>
+          <t>Paint</t>
+        </is>
+      </c>
+      <c r="D13" s="3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E13" s="3" t="n">
+        <v>9845069988</v>
+      </c>
+      <c r="F13" s="3" t="inlineStr">
+        <is>
+          <t>2020-08-03;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="12.8" customHeight="1" s="4">
+      <c r="A14" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="inlineStr">
+        <is>
+          <t>Aakash</t>
+        </is>
+      </c>
+      <c r="C14" s="3" t="inlineStr">
+        <is>
+          <t>Grains</t>
+        </is>
+      </c>
+      <c r="D14" s="3" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E14" s="3" t="n">
+        <v>9847081990</v>
+      </c>
+      <c r="F14" s="3" t="inlineStr">
+        <is>
+          <t>2020-08-03;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="15" ht="12.8" customHeight="1" s="4">
+      <c r="A15" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3" t="inlineStr">
+        <is>
+          <t>Akshita</t>
+        </is>
+      </c>
+      <c r="C15" s="3" t="inlineStr">
+        <is>
+          <t>Paint</t>
+        </is>
+      </c>
+      <c r="D15" s="3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E15" s="3" t="n">
+        <v>9845069988</v>
+      </c>
+      <c r="F15" s="3" t="inlineStr">
+        <is>
+          <t>2020-08-03;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="16" ht="12.8" customHeight="1" s="4">
+      <c r="A16" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3" t="inlineStr">
         <is>
           <t>aakash</t>
         </is>
       </c>
-      <c r="C8" s="2" t="inlineStr">
+      <c r="C16" s="3" t="inlineStr">
         <is>
           <t>fish</t>
         </is>
       </c>
-      <c r="D8" s="2" t="n">
+      <c r="D16" s="3" t="n">
         <v>10000000</v>
       </c>
-      <c r="E8" s="2" t="n">
+      <c r="E16" s="3" t="n">
         <v>9847081990</v>
       </c>
-    </row>
-    <row r="9" ht="12.8" customHeight="1" s="3">
-      <c r="A9" s="2" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2" t="inlineStr">
-        <is>
-          <t>psycoder01</t>
-        </is>
-      </c>
-      <c r="C9" s="2" t="inlineStr">
-        <is>
-          <t>laptop</t>
-        </is>
-      </c>
-      <c r="D9" s="2" t="n">
+      <c r="F16" s="3" t="inlineStr">
+        <is>
+          <t>2020-08-03;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="17" ht="12.8" customHeight="1" s="4">
+      <c r="A17" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3" t="inlineStr">
+        <is>
+          <t>Akshita</t>
+        </is>
+      </c>
+      <c r="C17" s="3" t="inlineStr">
+        <is>
+          <t>Paint</t>
+        </is>
+      </c>
+      <c r="D17" s="3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E17" s="3" t="n">
+        <v>9845069988</v>
+      </c>
+      <c r="F17" s="3" t="inlineStr">
+        <is>
+          <t>2020-08-03;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="18" ht="12.8" customHeight="1" s="4">
+      <c r="A18" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3" t="inlineStr">
+        <is>
+          <t>Aakash</t>
+        </is>
+      </c>
+      <c r="C18" s="3" t="inlineStr">
+        <is>
+          <t>Grains</t>
+        </is>
+      </c>
+      <c r="D18" s="3" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E18" s="3" t="n">
+        <v>9847081990</v>
+      </c>
+      <c r="F18" s="5" t="inlineStr">
+        <is>
+          <t>2020-08-04;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="19" ht="12.8" customHeight="1" s="4">
+      <c r="A19" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3" t="inlineStr">
+        <is>
+          <t>Akshita</t>
+        </is>
+      </c>
+      <c r="C19" s="3" t="inlineStr">
+        <is>
+          <t>Paint</t>
+        </is>
+      </c>
+      <c r="D19" s="3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E19" s="3" t="n">
+        <v>9845069988</v>
+      </c>
+      <c r="F19" s="5" t="inlineStr">
+        <is>
+          <t>2020-08-04;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="20" ht="12.8" customHeight="1" s="4">
+      <c r="A20" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3" t="inlineStr">
+        <is>
+          <t>aakash</t>
+        </is>
+      </c>
+      <c r="C20" s="3" t="inlineStr">
+        <is>
+          <t>fish</t>
+        </is>
+      </c>
+      <c r="D20" s="3" t="n">
         <v>10000000</v>
       </c>
-      <c r="E9" s="2" t="n">
-        <v>6463464364</v>
-      </c>
-    </row>
+      <c r="E20" s="3" t="n">
+        <v>9847081990</v>
+      </c>
+      <c r="F20" s="5" t="inlineStr">
+        <is>
+          <t>2020-08-04;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="21" ht="12.8" customHeight="1" s="4">
+      <c r="A21" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3" t="inlineStr">
+        <is>
+          <t>Akshita</t>
+        </is>
+      </c>
+      <c r="C21" s="3" t="inlineStr">
+        <is>
+          <t>Paint</t>
+        </is>
+      </c>
+      <c r="D21" s="3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E21" s="3" t="n">
+        <v>9845069988</v>
+      </c>
+      <c r="F21" s="5" t="inlineStr">
+        <is>
+          <t>2020-08-05;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="22" ht="12.8" customHeight="1" s="4">
+      <c r="A22" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3" t="inlineStr">
+        <is>
+          <t>Akshita</t>
+        </is>
+      </c>
+      <c r="C22" s="3" t="inlineStr">
+        <is>
+          <t>Paint</t>
+        </is>
+      </c>
+      <c r="D22" s="3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E22" s="3" t="n">
+        <v>9845069988</v>
+      </c>
+      <c r="F22" s="5" t="inlineStr">
+        <is>
+          <t>2020-08-05;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="23" ht="12.8" customHeight="1" s="4">
+      <c r="A23" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3" t="inlineStr">
+        <is>
+          <t>aakash</t>
+        </is>
+      </c>
+      <c r="C23" s="3" t="inlineStr">
+        <is>
+          <t>fish</t>
+        </is>
+      </c>
+      <c r="D23" s="3" t="n">
+        <v>10000000</v>
+      </c>
+      <c r="E23" s="3" t="n">
+        <v>9847081990</v>
+      </c>
+      <c r="F23" s="5" t="inlineStr">
+        <is>
+          <t>2020-08-05;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="24" ht="12.8" customHeight="1" s="4">
+      <c r="A24" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="3" t="inlineStr">
+        <is>
+          <t>Akshita</t>
+        </is>
+      </c>
+      <c r="C24" s="3" t="inlineStr">
+        <is>
+          <t>Paint</t>
+        </is>
+      </c>
+      <c r="D24" s="3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E24" s="3" t="n">
+        <v>9845069988</v>
+      </c>
+      <c r="F24" s="5" t="inlineStr">
+        <is>
+          <t>2020-08-05;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="25" ht="12.8" customHeight="1" s="4">
+      <c r="A25" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="3" t="inlineStr">
+        <is>
+          <t>Akshita</t>
+        </is>
+      </c>
+      <c r="C25" s="3" t="inlineStr">
+        <is>
+          <t>Paint</t>
+        </is>
+      </c>
+      <c r="D25" s="3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E25" s="3" t="n">
+        <v>9845069988</v>
+      </c>
+      <c r="F25" s="5" t="inlineStr">
+        <is>
+          <t>2020-08-05;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="26" ht="12.8" customHeight="1" s="4">
+      <c r="A26" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="3" t="inlineStr">
+        <is>
+          <t>Akshita</t>
+        </is>
+      </c>
+      <c r="C26" s="3" t="inlineStr">
+        <is>
+          <t>Paint</t>
+        </is>
+      </c>
+      <c r="D26" s="3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E26" s="3" t="n">
+        <v>9845069988</v>
+      </c>
+      <c r="F26" s="5" t="inlineStr">
+        <is>
+          <t>2020-08-05;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="27" ht="12.8" customHeight="1" s="4">
+      <c r="A27" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="3" t="inlineStr">
+        <is>
+          <t>Aakash</t>
+        </is>
+      </c>
+      <c r="C27" s="3" t="inlineStr">
+        <is>
+          <t>Grains</t>
+        </is>
+      </c>
+      <c r="D27" s="3" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E27" s="3" t="n">
+        <v>9847081990</v>
+      </c>
+      <c r="F27" s="5" t="inlineStr">
+        <is>
+          <t>2020-08-05;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="28" ht="12.8" customHeight="1" s="4">
+      <c r="A28" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="3" t="inlineStr">
+        <is>
+          <t>Akshita</t>
+        </is>
+      </c>
+      <c r="C28" s="3" t="inlineStr">
+        <is>
+          <t>Paint</t>
+        </is>
+      </c>
+      <c r="D28" s="3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E28" s="3" t="n">
+        <v>9845069988</v>
+      </c>
+      <c r="F28" s="5" t="inlineStr">
+        <is>
+          <t>2020-08-05;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="29" ht="12.8" customHeight="1" s="4">
+      <c r="A29" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="3" t="inlineStr">
+        <is>
+          <t>Aakash</t>
+        </is>
+      </c>
+      <c r="C29" s="3" t="inlineStr">
+        <is>
+          <t>Grains</t>
+        </is>
+      </c>
+      <c r="D29" s="3" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E29" s="3" t="n">
+        <v>9847081990</v>
+      </c>
+      <c r="F29" s="5" t="inlineStr">
+        <is>
+          <t>2020-08-05;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="30" ht="12.8" customHeight="1" s="4">
+      <c r="A30" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="3" t="inlineStr">
+        <is>
+          <t>Akshita</t>
+        </is>
+      </c>
+      <c r="C30" s="3" t="inlineStr">
+        <is>
+          <t>Paint</t>
+        </is>
+      </c>
+      <c r="D30" s="3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E30" s="3" t="n">
+        <v>9845069988</v>
+      </c>
+      <c r="F30" s="5" t="inlineStr">
+        <is>
+          <t>2020-08-05;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="31" ht="12.8" customHeight="1" s="4">
+      <c r="A31" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="3" t="inlineStr">
+        <is>
+          <t>aakash</t>
+        </is>
+      </c>
+      <c r="C31" s="3" t="inlineStr">
+        <is>
+          <t>fish</t>
+        </is>
+      </c>
+      <c r="D31" s="3" t="n">
+        <v>10000000</v>
+      </c>
+      <c r="E31" s="3" t="n">
+        <v>9847081990</v>
+      </c>
+      <c r="F31" s="5" t="inlineStr">
+        <is>
+          <t>2020-08-05;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="32" ht="12.8" customHeight="1" s="4">
+      <c r="A32" s="3" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="3" t="inlineStr">
+        <is>
+          <t>Aakash</t>
+        </is>
+      </c>
+      <c r="C32" s="3" t="inlineStr">
+        <is>
+          <t>Grains</t>
+        </is>
+      </c>
+      <c r="D32" s="3" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E32" s="3" t="n">
+        <v>9847081990</v>
+      </c>
+      <c r="F32" s="5" t="inlineStr">
+        <is>
+          <t>2020-08-05;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="33" ht="12.8" customHeight="1" s="4">
+      <c r="A33" s="3" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="3" t="inlineStr">
+        <is>
+          <t>Akshita</t>
+        </is>
+      </c>
+      <c r="C33" s="3" t="inlineStr">
+        <is>
+          <t>Paint</t>
+        </is>
+      </c>
+      <c r="D33" s="3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E33" s="3" t="n">
+        <v>9845069988</v>
+      </c>
+      <c r="F33" s="5" t="inlineStr">
+        <is>
+          <t>2020-08-05;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="34" ht="12.8" customHeight="1" s="4">
+      <c r="A34" s="3" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="3" t="inlineStr">
+        <is>
+          <t>Aakash</t>
+        </is>
+      </c>
+      <c r="C34" s="3" t="inlineStr">
+        <is>
+          <t>Grains</t>
+        </is>
+      </c>
+      <c r="D34" s="3" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E34" s="3" t="n">
+        <v>28357328535</v>
+      </c>
+      <c r="F34" s="5" t="inlineStr">
+        <is>
+          <t>2020-08-05;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="35" ht="12.8" customHeight="1" s="4">
+      <c r="A35" s="3" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="3" t="inlineStr">
+        <is>
+          <t>datetesting</t>
+        </is>
+      </c>
+      <c r="C35" s="3" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="D35" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="E35" s="3" t="n">
+        <v>325325325</v>
+      </c>
+      <c r="F35" s="3" t="inlineStr">
+        <is>
+          <t>2020-08-06;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="36" ht="12.8" customHeight="1" s="4"/>
+    <row r="37" ht="12.8" customHeight="1" s="4"/>
+    <row r="38" ht="12.8" customHeight="1" s="4"/>
+    <row r="39" ht="12.8" customHeight="1" s="4"/>
+    <row r="40" ht="12.8" customHeight="1" s="4"/>
+    <row r="41" ht="12.8" customHeight="1" s="4"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -911,126 +1651,803 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="F34" activeCellId="0" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col width="11.69" customWidth="1" style="2" min="1" max="64"/>
+    <col width="11.69" customWidth="1" style="3" min="1" max="5"/>
+    <col width="17.4" customWidth="1" style="3" min="6" max="6"/>
+    <col width="11.69" customWidth="1" style="3" min="7" max="64"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12.8" customHeight="1" s="3">
-      <c r="A1" s="2" t="inlineStr">
+    <row r="1" ht="12.8" customHeight="1" s="4">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>S.N</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>Product</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>Phone No</t>
         </is>
       </c>
-    </row>
-    <row r="2" ht="12.8" customHeight="1" s="3">
-      <c r="A2" s="2" t="n">
+      <c r="F1" s="3" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="12.8" customHeight="1" s="4">
+      <c r="A2" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>Akshita</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="inlineStr">
-        <is>
-          <t>Paint</t>
-        </is>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>2000</v>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>9845069988</v>
-      </c>
-    </row>
-    <row r="3" ht="12.8" customHeight="1" s="3">
-      <c r="A3" s="2" t="n">
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>Akshita</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>Paint</t>
+        </is>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>9845069988</v>
+      </c>
+      <c r="F2" s="3" t="inlineStr">
+        <is>
+          <t>2020-08-01;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="12.8" customHeight="1" s="4">
+      <c r="A3" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="inlineStr">
+      <c r="B3" s="3" t="inlineStr">
         <is>
           <t>Aakash</t>
         </is>
       </c>
-      <c r="C3" s="2" t="inlineStr">
+      <c r="C3" s="3" t="inlineStr">
         <is>
           <t>Grains</t>
         </is>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="D3" s="3" t="n">
         <v>1000</v>
       </c>
-      <c r="E3" s="2" t="n">
+      <c r="E3" s="3" t="n">
         <v>9847081990</v>
       </c>
-    </row>
-    <row r="4" ht="12.8" customHeight="1" s="3">
-      <c r="A4" s="2" t="n">
+      <c r="F3" s="3" t="inlineStr">
+        <is>
+          <t>2020-08-01;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="12.8" customHeight="1" s="4">
+      <c r="A4" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>Akshita</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>Paint</t>
-        </is>
-      </c>
-      <c r="D4" s="2" t="n">
-        <v>2000</v>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>9845069988</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="n">
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>Akshita</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>Paint</t>
+        </is>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>9845069988</v>
+      </c>
+      <c r="F4" s="3" t="inlineStr">
+        <is>
+          <t>2020-08-01;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="12.8" customHeight="1" s="4">
+      <c r="A5" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="inlineStr">
+      <c r="B5" s="3" t="inlineStr">
         <is>
           <t>aakash</t>
         </is>
       </c>
-      <c r="C5" s="2" t="inlineStr">
+      <c r="C5" s="3" t="inlineStr">
         <is>
           <t>fish</t>
         </is>
       </c>
-      <c r="D5" s="2" t="n">
+      <c r="D5" s="3" t="n">
         <v>1000</v>
       </c>
-      <c r="E5" s="2" t="n">
+      <c r="E5" s="3" t="n">
         <v>1094124214</v>
+      </c>
+      <c r="F5" s="3" t="inlineStr">
+        <is>
+          <t>2020-08-01;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="12.8" customHeight="1" s="4">
+      <c r="A6" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>Akshita</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="inlineStr">
+        <is>
+          <t>Paint</t>
+        </is>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>9845069988</v>
+      </c>
+      <c r="F6" s="3" t="inlineStr">
+        <is>
+          <t>2020-08-01;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="12.8" customHeight="1" s="4">
+      <c r="A7" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>Aakash</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="inlineStr">
+        <is>
+          <t>Grains</t>
+        </is>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E7" s="3" t="n">
+        <v>9847081990</v>
+      </c>
+      <c r="F7" s="3" t="inlineStr">
+        <is>
+          <t>2020-08-02;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="12.8" customHeight="1" s="4">
+      <c r="A8" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="inlineStr">
+        <is>
+          <t>Akshita</t>
+        </is>
+      </c>
+      <c r="C8" s="3" t="inlineStr">
+        <is>
+          <t>Paint</t>
+        </is>
+      </c>
+      <c r="D8" s="3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E8" s="3" t="n">
+        <v>9845069988</v>
+      </c>
+      <c r="F8" s="3" t="inlineStr">
+        <is>
+          <t>2020-08-02;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="12.8" customHeight="1" s="4">
+      <c r="A9" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>aakash</t>
+        </is>
+      </c>
+      <c r="C9" s="3" t="inlineStr">
+        <is>
+          <t>fish</t>
+        </is>
+      </c>
+      <c r="D9" s="3" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E9" s="3" t="n">
+        <v>1094124214</v>
+      </c>
+      <c r="F9" s="3" t="inlineStr">
+        <is>
+          <t>2020-08-02;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" ht="12.8" customHeight="1" s="4">
+      <c r="A10" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>Akshita</t>
+        </is>
+      </c>
+      <c r="C10" s="3" t="inlineStr">
+        <is>
+          <t>Paint</t>
+        </is>
+      </c>
+      <c r="D10" s="3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E10" s="3" t="n">
+        <v>9845069988</v>
+      </c>
+      <c r="F10" s="3" t="inlineStr">
+        <is>
+          <t>2020-08-03;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" ht="12.8" customHeight="1" s="4">
+      <c r="A11" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>Aakash</t>
+        </is>
+      </c>
+      <c r="C11" s="3" t="inlineStr">
+        <is>
+          <t>Grains</t>
+        </is>
+      </c>
+      <c r="D11" s="3" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E11" s="3" t="n">
+        <v>9847081990</v>
+      </c>
+      <c r="F11" s="3" t="inlineStr">
+        <is>
+          <t>2020-08-03;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" ht="12.8" customHeight="1" s="4">
+      <c r="A12" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>Akshita</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="inlineStr">
+        <is>
+          <t>Paint</t>
+        </is>
+      </c>
+      <c r="D12" s="3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E12" s="3" t="n">
+        <v>9845069988</v>
+      </c>
+      <c r="F12" s="3" t="inlineStr">
+        <is>
+          <t>2020-08-03;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="13" ht="12.8" customHeight="1" s="4">
+      <c r="A13" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="inlineStr">
+        <is>
+          <t>aakash</t>
+        </is>
+      </c>
+      <c r="C13" s="3" t="inlineStr">
+        <is>
+          <t>fish</t>
+        </is>
+      </c>
+      <c r="D13" s="3" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E13" s="3" t="n">
+        <v>1094124214</v>
+      </c>
+      <c r="F13" s="3" t="inlineStr">
+        <is>
+          <t>2020-08-03;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="12.8" customHeight="1" s="4">
+      <c r="A14" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="inlineStr">
+        <is>
+          <t>Akshita</t>
+        </is>
+      </c>
+      <c r="C14" s="3" t="inlineStr">
+        <is>
+          <t>Paint</t>
+        </is>
+      </c>
+      <c r="D14" s="3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E14" s="3" t="n">
+        <v>9845069988</v>
+      </c>
+      <c r="F14" s="3" t="inlineStr">
+        <is>
+          <t>2020-08-03;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="15" ht="12.8" customHeight="1" s="4">
+      <c r="A15" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3" t="inlineStr">
+        <is>
+          <t>Aakash</t>
+        </is>
+      </c>
+      <c r="C15" s="3" t="inlineStr">
+        <is>
+          <t>Grains</t>
+        </is>
+      </c>
+      <c r="D15" s="3" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E15" s="3" t="n">
+        <v>9847081990</v>
+      </c>
+      <c r="F15" s="3" t="inlineStr">
+        <is>
+          <t>2020-08-03;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="16" ht="12.8" customHeight="1" s="4">
+      <c r="A16" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3" t="inlineStr">
+        <is>
+          <t>Akshita</t>
+        </is>
+      </c>
+      <c r="C16" s="3" t="inlineStr">
+        <is>
+          <t>Paint</t>
+        </is>
+      </c>
+      <c r="D16" s="3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E16" s="3" t="n">
+        <v>9845069988</v>
+      </c>
+      <c r="F16" s="3" t="inlineStr">
+        <is>
+          <t>2020-08-03;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="17" ht="12.8" customHeight="1" s="4">
+      <c r="A17" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3" t="inlineStr">
+        <is>
+          <t>aakash</t>
+        </is>
+      </c>
+      <c r="C17" s="3" t="inlineStr">
+        <is>
+          <t>fish</t>
+        </is>
+      </c>
+      <c r="D17" s="3" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E17" s="3" t="n">
+        <v>1094124214</v>
+      </c>
+      <c r="F17" s="3" t="inlineStr">
+        <is>
+          <t>2020-08-03;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="18" ht="12.8" customHeight="1" s="4">
+      <c r="A18" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3" t="inlineStr">
+        <is>
+          <t>Akshita</t>
+        </is>
+      </c>
+      <c r="C18" s="3" t="inlineStr">
+        <is>
+          <t>Paint</t>
+        </is>
+      </c>
+      <c r="D18" s="3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E18" s="3" t="n">
+        <v>9845069988</v>
+      </c>
+      <c r="F18" s="3" t="inlineStr">
+        <is>
+          <t>2020-08-03;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="19" ht="12.8" customHeight="1" s="4">
+      <c r="A19" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3" t="inlineStr">
+        <is>
+          <t>Aakash</t>
+        </is>
+      </c>
+      <c r="C19" s="3" t="inlineStr">
+        <is>
+          <t>Grains</t>
+        </is>
+      </c>
+      <c r="D19" s="3" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E19" s="3" t="n">
+        <v>9847081990</v>
+      </c>
+      <c r="F19" s="5" t="inlineStr">
+        <is>
+          <t>2020-08-04;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="20" ht="12.8" customHeight="1" s="4">
+      <c r="A20" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3" t="inlineStr">
+        <is>
+          <t>Akshita</t>
+        </is>
+      </c>
+      <c r="C20" s="3" t="inlineStr">
+        <is>
+          <t>Paint</t>
+        </is>
+      </c>
+      <c r="D20" s="3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E20" s="3" t="n">
+        <v>9845069988</v>
+      </c>
+      <c r="F20" s="5" t="inlineStr">
+        <is>
+          <t>2020-08-04;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="21" ht="12.8" customHeight="1" s="4">
+      <c r="A21" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3" t="inlineStr">
+        <is>
+          <t>aakash</t>
+        </is>
+      </c>
+      <c r="C21" s="3" t="inlineStr">
+        <is>
+          <t>fish</t>
+        </is>
+      </c>
+      <c r="D21" s="3" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E21" s="3" t="n">
+        <v>1094124214</v>
+      </c>
+      <c r="F21" s="5" t="inlineStr">
+        <is>
+          <t>2020-08-04;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="22" ht="12.8" customHeight="1" s="4">
+      <c r="A22" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3" t="inlineStr">
+        <is>
+          <t>Akshita</t>
+        </is>
+      </c>
+      <c r="C22" s="3" t="inlineStr">
+        <is>
+          <t>Paint</t>
+        </is>
+      </c>
+      <c r="D22" s="3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E22" s="3" t="n">
+        <v>9845069988</v>
+      </c>
+      <c r="F22" s="5" t="inlineStr">
+        <is>
+          <t>2020-08-05;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="23" ht="12.8" customHeight="1" s="4">
+      <c r="A23" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3" t="inlineStr">
+        <is>
+          <t>Aakash</t>
+        </is>
+      </c>
+      <c r="C23" s="3" t="inlineStr">
+        <is>
+          <t>Grains</t>
+        </is>
+      </c>
+      <c r="D23" s="3" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E23" s="3" t="n">
+        <v>9847081990</v>
+      </c>
+      <c r="F23" s="5" t="inlineStr">
+        <is>
+          <t>2020-08-05;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="24" ht="12.8" customHeight="1" s="4">
+      <c r="A24" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="3" t="inlineStr">
+        <is>
+          <t>Akshita</t>
+        </is>
+      </c>
+      <c r="C24" s="3" t="inlineStr">
+        <is>
+          <t>Paint</t>
+        </is>
+      </c>
+      <c r="D24" s="3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E24" s="3" t="n">
+        <v>9845069988</v>
+      </c>
+      <c r="F24" s="5" t="inlineStr">
+        <is>
+          <t>2020-08-05;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="25" ht="12.8" customHeight="1" s="4">
+      <c r="A25" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="3" t="inlineStr">
+        <is>
+          <t>Akshita</t>
+        </is>
+      </c>
+      <c r="C25" s="3" t="inlineStr">
+        <is>
+          <t>Paint</t>
+        </is>
+      </c>
+      <c r="D25" s="3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E25" s="3" t="n">
+        <v>9845069988</v>
+      </c>
+      <c r="F25" s="5" t="inlineStr">
+        <is>
+          <t>2020-08-05;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="26" ht="12.8" customHeight="1" s="4">
+      <c r="A26" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="3" t="inlineStr">
+        <is>
+          <t>Aakash</t>
+        </is>
+      </c>
+      <c r="C26" s="3" t="inlineStr">
+        <is>
+          <t>Grains</t>
+        </is>
+      </c>
+      <c r="D26" s="3" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E26" s="3" t="n">
+        <v>9847081990</v>
+      </c>
+      <c r="F26" s="5" t="inlineStr">
+        <is>
+          <t>2020-08-05;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="27" ht="12.8" customHeight="1" s="4">
+      <c r="A27" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="3" t="inlineStr">
+        <is>
+          <t>Akshita</t>
+        </is>
+      </c>
+      <c r="C27" s="3" t="inlineStr">
+        <is>
+          <t>Paint</t>
+        </is>
+      </c>
+      <c r="D27" s="3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E27" s="3" t="n">
+        <v>9845069988</v>
+      </c>
+      <c r="F27" s="5" t="inlineStr">
+        <is>
+          <t>2020-08-05;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="28" ht="12.8" customHeight="1" s="4">
+      <c r="A28" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="3" t="inlineStr">
+        <is>
+          <t>aakash</t>
+        </is>
+      </c>
+      <c r="C28" s="3" t="inlineStr">
+        <is>
+          <t>fish</t>
+        </is>
+      </c>
+      <c r="D28" s="3" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E28" s="3" t="n">
+        <v>1094124214</v>
+      </c>
+      <c r="F28" s="5" t="inlineStr">
+        <is>
+          <t>2020-08-05;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="29" ht="12.8" customHeight="1" s="4">
+      <c r="A29" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="3" t="inlineStr">
+        <is>
+          <t>aman</t>
+        </is>
+      </c>
+      <c r="C29" s="3" t="inlineStr">
+        <is>
+          <t>eggs</t>
+        </is>
+      </c>
+      <c r="D29" s="3" t="n">
+        <v>2000</v>
+      </c>
+      <c r="E29" s="3" t="n">
+        <v>35325533325</v>
+      </c>
+      <c r="F29" s="5" t="inlineStr">
+        <is>
+          <t>2020-08-06;16-09</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="3" t="inlineStr">
+        <is>
+          <t>testdateex</t>
+        </is>
+      </c>
+      <c r="C30" s="3" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="D30" s="3" t="n">
+        <v>10000000</v>
+      </c>
+      <c r="E30" s="3" t="n">
+        <v>235325325</v>
+      </c>
+      <c r="F30" s="3" t="inlineStr">
+        <is>
+          <t>2020-08-06;16-16</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added analytics page and functions
</commit_message>
<xml_diff>
--- a/store/data.xlsx
+++ b/store/data.xlsx
@@ -608,7 +608,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="F28"/>
@@ -737,19 +737,19 @@
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>aakash</t>
+          <t>Akshita</t>
         </is>
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>fish</t>
+          <t>Paint</t>
         </is>
       </c>
       <c r="D5" s="2" t="n">
-        <v>10000000</v>
+        <v>2000</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>9847081990</v>
+        <v>9845069988</v>
       </c>
       <c r="F5" s="2" t="inlineStr">
         <is>
@@ -763,23 +763,23 @@
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>Akshita</t>
+          <t>Aakash</t>
         </is>
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>Paint</t>
+          <t>Grains</t>
         </is>
       </c>
       <c r="D6" s="2" t="n">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>9845069988</v>
+        <v>9847081990</v>
       </c>
       <c r="F6" s="2" t="inlineStr">
         <is>
-          <t>2020-08-01;16-09</t>
+          <t>2020-08-02;16-09</t>
         </is>
       </c>
     </row>
@@ -789,19 +789,19 @@
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>Aakash</t>
+          <t>Akshita</t>
         </is>
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>
-          <t>Grains</t>
+          <t>Paint</t>
         </is>
       </c>
       <c r="D7" s="2" t="n">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>9847081990</v>
+        <v>9845069988</v>
       </c>
       <c r="F7" s="2" t="inlineStr">
         <is>
@@ -809,734 +809,34 @@
         </is>
       </c>
     </row>
-    <row r="8" ht="12.8" customHeight="1" s="3">
-      <c r="A8" s="2" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="inlineStr">
-        <is>
-          <t>Akshita</t>
-        </is>
-      </c>
-      <c r="C8" s="2" t="inlineStr">
-        <is>
-          <t>Paint</t>
-        </is>
-      </c>
-      <c r="D8" s="2" t="n">
-        <v>2000</v>
-      </c>
-      <c r="E8" s="2" t="n">
-        <v>9845069988</v>
-      </c>
-      <c r="F8" s="2" t="inlineStr">
-        <is>
-          <t>2020-08-02;16-09</t>
-        </is>
-      </c>
-    </row>
-    <row r="9" ht="12.8" customHeight="1" s="3">
-      <c r="A9" s="2" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2" t="inlineStr">
-        <is>
-          <t>aakash</t>
-        </is>
-      </c>
-      <c r="C9" s="2" t="inlineStr">
-        <is>
-          <t>fish</t>
-        </is>
-      </c>
-      <c r="D9" s="2" t="n">
-        <v>10000000</v>
-      </c>
-      <c r="E9" s="2" t="n">
-        <v>9847081990</v>
-      </c>
-      <c r="F9" s="2" t="inlineStr">
-        <is>
-          <t>2020-08-02;16-09</t>
-        </is>
-      </c>
-    </row>
-    <row r="10" ht="12.8" customHeight="1" s="3">
-      <c r="A10" s="2" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2" t="inlineStr">
-        <is>
-          <t>Akshita</t>
-        </is>
-      </c>
-      <c r="C10" s="2" t="inlineStr">
-        <is>
-          <t>Paint</t>
-        </is>
-      </c>
-      <c r="D10" s="2" t="n">
-        <v>2000</v>
-      </c>
-      <c r="E10" s="2" t="n">
-        <v>9845069988</v>
-      </c>
-      <c r="F10" s="2" t="inlineStr">
-        <is>
-          <t>2020-08-03;16-09</t>
-        </is>
-      </c>
-    </row>
-    <row r="11" ht="12.8" customHeight="1" s="3">
-      <c r="A11" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2" t="inlineStr">
-        <is>
-          <t>Aakash</t>
-        </is>
-      </c>
-      <c r="C11" s="2" t="inlineStr">
-        <is>
-          <t>Grains</t>
-        </is>
-      </c>
-      <c r="D11" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="E11" s="2" t="n">
-        <v>9847081990</v>
-      </c>
-      <c r="F11" s="2" t="inlineStr">
-        <is>
-          <t>2020-08-03;16-09</t>
-        </is>
-      </c>
-    </row>
-    <row r="12" ht="12.8" customHeight="1" s="3">
-      <c r="A12" s="2" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" s="2" t="inlineStr">
-        <is>
-          <t>Akshita</t>
-        </is>
-      </c>
-      <c r="C12" s="2" t="inlineStr">
-        <is>
-          <t>Paint</t>
-        </is>
-      </c>
-      <c r="D12" s="2" t="n">
-        <v>2000</v>
-      </c>
-      <c r="E12" s="2" t="n">
-        <v>9845069988</v>
-      </c>
-      <c r="F12" s="2" t="inlineStr">
-        <is>
-          <t>2020-08-03;16-09</t>
-        </is>
-      </c>
-    </row>
-    <row r="13" ht="12.8" customHeight="1" s="3">
-      <c r="A13" s="2" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2" t="inlineStr">
-        <is>
-          <t>Akshita</t>
-        </is>
-      </c>
-      <c r="C13" s="2" t="inlineStr">
-        <is>
-          <t>Paint</t>
-        </is>
-      </c>
-      <c r="D13" s="2" t="n">
-        <v>2000</v>
-      </c>
-      <c r="E13" s="2" t="n">
-        <v>9845069988</v>
-      </c>
-      <c r="F13" s="2" t="inlineStr">
-        <is>
-          <t>2020-08-03;16-09</t>
-        </is>
-      </c>
-    </row>
-    <row r="14" ht="12.8" customHeight="1" s="3">
-      <c r="A14" s="2" t="n">
-        <v>13</v>
-      </c>
-      <c r="B14" s="2" t="inlineStr">
-        <is>
-          <t>Aakash</t>
-        </is>
-      </c>
-      <c r="C14" s="2" t="inlineStr">
-        <is>
-          <t>Grains</t>
-        </is>
-      </c>
-      <c r="D14" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="E14" s="2" t="n">
-        <v>9847081990</v>
-      </c>
-      <c r="F14" s="2" t="inlineStr">
-        <is>
-          <t>2020-08-03;16-09</t>
-        </is>
-      </c>
-    </row>
-    <row r="15" ht="12.8" customHeight="1" s="3">
-      <c r="A15" s="2" t="n">
-        <v>14</v>
-      </c>
-      <c r="B15" s="2" t="inlineStr">
-        <is>
-          <t>Akshita</t>
-        </is>
-      </c>
-      <c r="C15" s="2" t="inlineStr">
-        <is>
-          <t>Paint</t>
-        </is>
-      </c>
-      <c r="D15" s="2" t="n">
-        <v>2000</v>
-      </c>
-      <c r="E15" s="2" t="n">
-        <v>9845069988</v>
-      </c>
-      <c r="F15" s="2" t="inlineStr">
-        <is>
-          <t>2020-08-03;16-09</t>
-        </is>
-      </c>
-    </row>
-    <row r="16" ht="12.8" customHeight="1" s="3">
-      <c r="A16" s="2" t="n">
-        <v>15</v>
-      </c>
-      <c r="B16" s="2" t="inlineStr">
-        <is>
-          <t>aakash</t>
-        </is>
-      </c>
-      <c r="C16" s="2" t="inlineStr">
-        <is>
-          <t>fish</t>
-        </is>
-      </c>
-      <c r="D16" s="2" t="n">
-        <v>10000000</v>
-      </c>
-      <c r="E16" s="2" t="n">
-        <v>9847081990</v>
-      </c>
-      <c r="F16" s="2" t="inlineStr">
-        <is>
-          <t>2020-08-03;16-09</t>
-        </is>
-      </c>
-    </row>
-    <row r="17" ht="12.8" customHeight="1" s="3">
-      <c r="A17" s="2" t="n">
-        <v>16</v>
-      </c>
-      <c r="B17" s="2" t="inlineStr">
-        <is>
-          <t>Akshita</t>
-        </is>
-      </c>
-      <c r="C17" s="2" t="inlineStr">
-        <is>
-          <t>Paint</t>
-        </is>
-      </c>
-      <c r="D17" s="2" t="n">
-        <v>2000</v>
-      </c>
-      <c r="E17" s="2" t="n">
-        <v>9845069988</v>
-      </c>
-      <c r="F17" s="2" t="inlineStr">
-        <is>
-          <t>2020-08-03;16-09</t>
-        </is>
-      </c>
-    </row>
-    <row r="18" ht="12.8" customHeight="1" s="3">
-      <c r="A18" s="2" t="n">
-        <v>17</v>
-      </c>
-      <c r="B18" s="2" t="inlineStr">
-        <is>
-          <t>Aakash</t>
-        </is>
-      </c>
-      <c r="C18" s="2" t="inlineStr">
-        <is>
-          <t>Grains</t>
-        </is>
-      </c>
-      <c r="D18" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="E18" s="2" t="n">
-        <v>9847081990</v>
-      </c>
-      <c r="F18" s="2" t="inlineStr">
-        <is>
-          <t>2020-08-04;16-09</t>
-        </is>
-      </c>
-    </row>
-    <row r="19" ht="12.8" customHeight="1" s="3">
-      <c r="A19" s="2" t="n">
-        <v>18</v>
-      </c>
-      <c r="B19" s="2" t="inlineStr">
-        <is>
-          <t>Akshita</t>
-        </is>
-      </c>
-      <c r="C19" s="2" t="inlineStr">
-        <is>
-          <t>Paint</t>
-        </is>
-      </c>
-      <c r="D19" s="2" t="n">
-        <v>2000</v>
-      </c>
-      <c r="E19" s="2" t="n">
-        <v>9845069988</v>
-      </c>
-      <c r="F19" s="2" t="inlineStr">
-        <is>
-          <t>2020-08-04;16-09</t>
-        </is>
-      </c>
-    </row>
-    <row r="20" ht="12.8" customHeight="1" s="3">
-      <c r="A20" s="2" t="n">
-        <v>19</v>
-      </c>
-      <c r="B20" s="2" t="inlineStr">
-        <is>
-          <t>aakash</t>
-        </is>
-      </c>
-      <c r="C20" s="2" t="inlineStr">
-        <is>
-          <t>fish</t>
-        </is>
-      </c>
-      <c r="D20" s="2" t="n">
-        <v>10000000</v>
-      </c>
-      <c r="E20" s="2" t="n">
-        <v>9847081990</v>
-      </c>
-      <c r="F20" s="2" t="inlineStr">
-        <is>
-          <t>2020-08-04;16-09</t>
-        </is>
-      </c>
-    </row>
-    <row r="21" ht="12.8" customHeight="1" s="3">
-      <c r="A21" s="2" t="n">
-        <v>20</v>
-      </c>
-      <c r="B21" s="2" t="inlineStr">
-        <is>
-          <t>Akshita</t>
-        </is>
-      </c>
-      <c r="C21" s="2" t="inlineStr">
-        <is>
-          <t>Paint</t>
-        </is>
-      </c>
-      <c r="D21" s="2" t="n">
-        <v>2000</v>
-      </c>
-      <c r="E21" s="2" t="n">
-        <v>9845069988</v>
-      </c>
-      <c r="F21" s="2" t="inlineStr">
-        <is>
-          <t>2020-08-05;16-09</t>
-        </is>
-      </c>
-    </row>
-    <row r="22" ht="12.8" customHeight="1" s="3">
-      <c r="A22" s="2" t="n">
-        <v>21</v>
-      </c>
-      <c r="B22" s="2" t="inlineStr">
-        <is>
-          <t>Akshita</t>
-        </is>
-      </c>
-      <c r="C22" s="2" t="inlineStr">
-        <is>
-          <t>Paint</t>
-        </is>
-      </c>
-      <c r="D22" s="2" t="n">
-        <v>2000</v>
-      </c>
-      <c r="E22" s="2" t="n">
-        <v>9845069988</v>
-      </c>
-      <c r="F22" s="2" t="inlineStr">
-        <is>
-          <t>2020-08-05;16-09</t>
-        </is>
-      </c>
-    </row>
-    <row r="23" ht="12.8" customHeight="1" s="3">
-      <c r="A23" s="2" t="n">
-        <v>22</v>
-      </c>
-      <c r="B23" s="2" t="inlineStr">
-        <is>
-          <t>aakash</t>
-        </is>
-      </c>
-      <c r="C23" s="2" t="inlineStr">
-        <is>
-          <t>fish</t>
-        </is>
-      </c>
-      <c r="D23" s="2" t="n">
-        <v>10000000</v>
-      </c>
-      <c r="E23" s="2" t="n">
-        <v>9847081990</v>
-      </c>
-      <c r="F23" s="2" t="inlineStr">
-        <is>
-          <t>2020-08-05;16-09</t>
-        </is>
-      </c>
-    </row>
-    <row r="24" ht="12.8" customHeight="1" s="3">
-      <c r="A24" s="2" t="n">
-        <v>23</v>
-      </c>
-      <c r="B24" s="2" t="inlineStr">
-        <is>
-          <t>Akshita</t>
-        </is>
-      </c>
-      <c r="C24" s="2" t="inlineStr">
-        <is>
-          <t>Paint</t>
-        </is>
-      </c>
-      <c r="D24" s="2" t="n">
-        <v>2000</v>
-      </c>
-      <c r="E24" s="2" t="n">
-        <v>9845069988</v>
-      </c>
-      <c r="F24" s="2" t="inlineStr">
-        <is>
-          <t>2020-08-05;16-09</t>
-        </is>
-      </c>
-    </row>
-    <row r="25" ht="12.8" customHeight="1" s="3">
-      <c r="A25" s="2" t="n">
-        <v>24</v>
-      </c>
-      <c r="B25" s="2" t="inlineStr">
-        <is>
-          <t>Akshita</t>
-        </is>
-      </c>
-      <c r="C25" s="2" t="inlineStr">
-        <is>
-          <t>Paint</t>
-        </is>
-      </c>
-      <c r="D25" s="2" t="n">
-        <v>2000</v>
-      </c>
-      <c r="E25" s="2" t="n">
-        <v>9845069988</v>
-      </c>
-      <c r="F25" s="2" t="inlineStr">
-        <is>
-          <t>2020-08-05;16-09</t>
-        </is>
-      </c>
-    </row>
-    <row r="26" ht="12.8" customHeight="1" s="3">
-      <c r="A26" s="2" t="n">
-        <v>25</v>
-      </c>
-      <c r="B26" s="2" t="inlineStr">
-        <is>
-          <t>Akshita</t>
-        </is>
-      </c>
-      <c r="C26" s="2" t="inlineStr">
-        <is>
-          <t>Paint</t>
-        </is>
-      </c>
-      <c r="D26" s="2" t="n">
-        <v>2000</v>
-      </c>
-      <c r="E26" s="2" t="n">
-        <v>9845069988</v>
-      </c>
-      <c r="F26" s="2" t="inlineStr">
-        <is>
-          <t>2020-08-05;16-09</t>
-        </is>
-      </c>
-    </row>
-    <row r="27" ht="12.8" customHeight="1" s="3">
-      <c r="A27" s="2" t="n">
-        <v>26</v>
-      </c>
-      <c r="B27" s="2" t="inlineStr">
-        <is>
-          <t>Aakash</t>
-        </is>
-      </c>
-      <c r="C27" s="2" t="inlineStr">
-        <is>
-          <t>Grains</t>
-        </is>
-      </c>
-      <c r="D27" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="E27" s="2" t="n">
-        <v>9847081990</v>
-      </c>
-      <c r="F27" s="2" t="inlineStr">
-        <is>
-          <t>2020-08-05;16-09</t>
-        </is>
-      </c>
-    </row>
-    <row r="28" ht="12.8" customHeight="1" s="3">
-      <c r="A28" s="2" t="n">
-        <v>27</v>
-      </c>
-      <c r="B28" s="2" t="inlineStr">
-        <is>
-          <t>Akshita</t>
-        </is>
-      </c>
-      <c r="C28" s="2" t="inlineStr">
-        <is>
-          <t>Paint</t>
-        </is>
-      </c>
-      <c r="D28" s="2" t="n">
-        <v>2000</v>
-      </c>
-      <c r="E28" s="2" t="n">
-        <v>9845069988</v>
-      </c>
-      <c r="F28" s="2" t="inlineStr">
-        <is>
-          <t>2020-08-05;16-09</t>
-        </is>
-      </c>
-    </row>
-    <row r="29" ht="12.8" customHeight="1" s="3">
-      <c r="A29" s="2" t="n">
-        <v>28</v>
-      </c>
-      <c r="B29" s="2" t="inlineStr">
-        <is>
-          <t>Aakash</t>
-        </is>
-      </c>
-      <c r="C29" s="2" t="inlineStr">
-        <is>
-          <t>Grains</t>
-        </is>
-      </c>
-      <c r="D29" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="E29" s="2" t="n">
-        <v>9847081990</v>
-      </c>
-      <c r="F29" s="2" t="inlineStr">
-        <is>
-          <t>2020-08-05;16-09</t>
-        </is>
-      </c>
-    </row>
-    <row r="30" ht="12.8" customHeight="1" s="3">
-      <c r="A30" s="2" t="n">
-        <v>29</v>
-      </c>
-      <c r="B30" s="2" t="inlineStr">
-        <is>
-          <t>Akshita</t>
-        </is>
-      </c>
-      <c r="C30" s="2" t="inlineStr">
-        <is>
-          <t>Paint</t>
-        </is>
-      </c>
-      <c r="D30" s="2" t="n">
-        <v>2000</v>
-      </c>
-      <c r="E30" s="2" t="n">
-        <v>9845069988</v>
-      </c>
-      <c r="F30" s="2" t="inlineStr">
-        <is>
-          <t>2020-08-05;16-09</t>
-        </is>
-      </c>
-    </row>
-    <row r="31" ht="12.8" customHeight="1" s="3">
-      <c r="A31" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="B31" s="2" t="inlineStr">
-        <is>
-          <t>aakash</t>
-        </is>
-      </c>
-      <c r="C31" s="2" t="inlineStr">
-        <is>
-          <t>fish</t>
-        </is>
-      </c>
-      <c r="D31" s="2" t="n">
-        <v>10000000</v>
-      </c>
-      <c r="E31" s="2" t="n">
-        <v>9847081990</v>
-      </c>
-      <c r="F31" s="2" t="inlineStr">
-        <is>
-          <t>2020-08-05;16-09</t>
-        </is>
-      </c>
-    </row>
-    <row r="32" ht="12.8" customHeight="1" s="3">
-      <c r="A32" s="2" t="n">
-        <v>31</v>
-      </c>
-      <c r="B32" s="2" t="inlineStr">
-        <is>
-          <t>Aakash</t>
-        </is>
-      </c>
-      <c r="C32" s="2" t="inlineStr">
-        <is>
-          <t>Grains</t>
-        </is>
-      </c>
-      <c r="D32" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="E32" s="2" t="n">
-        <v>9847081990</v>
-      </c>
-      <c r="F32" s="2" t="inlineStr">
-        <is>
-          <t>2020-08-05;16-09</t>
-        </is>
-      </c>
-    </row>
-    <row r="33" ht="12.8" customHeight="1" s="3">
-      <c r="A33" s="2" t="n">
-        <v>32</v>
-      </c>
-      <c r="B33" s="2" t="inlineStr">
-        <is>
-          <t>Akshita</t>
-        </is>
-      </c>
-      <c r="C33" s="2" t="inlineStr">
-        <is>
-          <t>Paint</t>
-        </is>
-      </c>
-      <c r="D33" s="2" t="n">
-        <v>2000</v>
-      </c>
-      <c r="E33" s="2" t="n">
-        <v>9845069988</v>
-      </c>
-      <c r="F33" s="2" t="inlineStr">
-        <is>
-          <t>2020-08-05;16-09</t>
-        </is>
-      </c>
-    </row>
-    <row r="34" ht="12.8" customHeight="1" s="3">
-      <c r="A34" s="2" t="n">
-        <v>33</v>
-      </c>
-      <c r="B34" s="2" t="inlineStr">
-        <is>
-          <t>Aakash</t>
-        </is>
-      </c>
-      <c r="C34" s="2" t="inlineStr">
-        <is>
-          <t>Grains</t>
-        </is>
-      </c>
-      <c r="D34" s="2" t="n">
-        <v>1000</v>
-      </c>
-      <c r="E34" s="2" t="n">
-        <v>28357328535</v>
-      </c>
-      <c r="F34" s="2" t="inlineStr">
-        <is>
-          <t>2020-08-05;16-09</t>
-        </is>
-      </c>
-    </row>
-    <row r="35" ht="12.8" customHeight="1" s="3">
-      <c r="A35" s="2" t="n">
-        <v>34</v>
-      </c>
-      <c r="B35" s="2" t="inlineStr">
-        <is>
-          <t>datetesting</t>
-        </is>
-      </c>
-      <c r="C35" s="2" t="inlineStr">
-        <is>
-          <t>date</t>
-        </is>
-      </c>
-      <c r="D35" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="E35" s="2" t="n">
-        <v>325325325</v>
-      </c>
-      <c r="F35" s="2" t="inlineStr">
-        <is>
-          <t>2020-08-06;16-09</t>
-        </is>
-      </c>
-    </row>
+    <row r="8" ht="12.8" customHeight="1" s="3"/>
+    <row r="9" ht="12.8" customHeight="1" s="3"/>
+    <row r="10" ht="12.8" customHeight="1" s="3"/>
+    <row r="11" ht="12.8" customHeight="1" s="3"/>
+    <row r="12" ht="12.8" customHeight="1" s="3"/>
+    <row r="13" ht="12.8" customHeight="1" s="3"/>
+    <row r="14" ht="12.8" customHeight="1" s="3"/>
+    <row r="15" ht="12.8" customHeight="1" s="3"/>
+    <row r="16" ht="12.8" customHeight="1" s="3"/>
+    <row r="17" ht="12.8" customHeight="1" s="3"/>
+    <row r="18" ht="12.8" customHeight="1" s="3"/>
+    <row r="19" ht="12.8" customHeight="1" s="3"/>
+    <row r="20" ht="12.8" customHeight="1" s="3"/>
+    <row r="21" ht="12.8" customHeight="1" s="3"/>
+    <row r="22" ht="12.8" customHeight="1" s="3"/>
+    <row r="23" ht="12.8" customHeight="1" s="3"/>
+    <row r="24" ht="12.8" customHeight="1" s="3"/>
+    <row r="25" ht="12.8" customHeight="1" s="3"/>
+    <row r="26" ht="12.8" customHeight="1" s="3"/>
+    <row r="27" ht="12.8" customHeight="1" s="3"/>
+    <row r="28" ht="12.8" customHeight="1" s="3"/>
+    <row r="29" ht="12.8" customHeight="1" s="3"/>
+    <row r="30" ht="12.8" customHeight="1" s="3"/>
+    <row r="31" ht="12.8" customHeight="1" s="3"/>
+    <row r="32" ht="12.8" customHeight="1" s="3"/>
+    <row r="33" ht="12.8" customHeight="1" s="3"/>
+    <row r="34" ht="12.8" customHeight="1" s="3"/>
+    <row r="35" ht="12.8" customHeight="1" s="3"/>
     <row r="36" ht="12.8" customHeight="1" s="3"/>
     <row r="37" ht="12.8" customHeight="1" s="3"/>
     <row r="38" ht="12.8" customHeight="1" s="3"/>
@@ -1564,7 +864,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F34" activeCellId="0" sqref="F34"/>
@@ -2311,58 +1611,8 @@
         </is>
       </c>
     </row>
-    <row r="29" ht="12.8" customHeight="1" s="3">
-      <c r="A29" s="2" t="n">
-        <v>28</v>
-      </c>
-      <c r="B29" s="2" t="inlineStr">
-        <is>
-          <t>aman</t>
-        </is>
-      </c>
-      <c r="C29" s="2" t="inlineStr">
-        <is>
-          <t>eggs</t>
-        </is>
-      </c>
-      <c r="D29" s="2" t="n">
-        <v>2000</v>
-      </c>
-      <c r="E29" s="2" t="n">
-        <v>35325533325</v>
-      </c>
-      <c r="F29" s="2" t="inlineStr">
-        <is>
-          <t>2020-08-06;16-09</t>
-        </is>
-      </c>
-    </row>
-    <row r="30" ht="12.8" customHeight="1" s="3">
-      <c r="A30" s="2" t="n">
-        <v>29</v>
-      </c>
-      <c r="B30" s="2" t="inlineStr">
-        <is>
-          <t>testdateex</t>
-        </is>
-      </c>
-      <c r="C30" s="2" t="inlineStr">
-        <is>
-          <t>date</t>
-        </is>
-      </c>
-      <c r="D30" s="2" t="n">
-        <v>10000000</v>
-      </c>
-      <c r="E30" s="2" t="n">
-        <v>235325325</v>
-      </c>
-      <c r="F30" s="2" t="inlineStr">
-        <is>
-          <t>2020-08-06;16-16</t>
-        </is>
-      </c>
-    </row>
+    <row r="29" ht="12.8" customHeight="1" s="3"/>
+    <row r="30" ht="12.8" customHeight="1" s="3"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>